<commit_message>
Distinct elements in window of size K
</commit_message>
<xml_diff>
--- a/Question Sheet.xlsx
+++ b/Question Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shubhammazumdar/Library/Mobile Documents/com~apple~CloudDocs/Level2/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AC96E5-3F29-FE40-A75E-DAFCBBB64B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F59C6E-2EBA-CD4F-AFC1-20F6B04D31F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15880" activeTab="1" xr2:uid="{688ABEC1-99B5-A148-B24E-133D3C1DE4DF}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15820" activeTab="1" xr2:uid="{688ABEC1-99B5-A148-B24E-133D3C1DE4DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="80">
   <si>
     <t>17th Aug 2022</t>
   </si>
@@ -274,6 +274,9 @@
   <si>
     <t>https://online-quzi-2.vercel.app/quiz</t>
   </si>
+  <si>
+    <t>Answers on 6th Sep class</t>
+  </si>
 </sst>
 </file>
 
@@ -320,7 +323,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -330,6 +333,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -347,7 +356,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -358,6 +367,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -675,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD82ACF5-6E46-2A4E-8CDB-3350DDC49501}">
   <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="132" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A6" zoomScale="132" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1100,7 +1110,7 @@
       <c r="D13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="8" t="s">
         <v>77</v>
       </c>
       <c r="F13" s="4"/>
@@ -1303,7 +1313,9 @@
       <c r="D19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="4"/>
+      <c r="E19" s="6" t="s">
+        <v>77</v>
+      </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
@@ -28311,20 +28323,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B700801-C5A7-E248-947B-370713DC0001}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>78</v>
+      </c>
+      <c r="B1" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
largest subarray with continuous element
</commit_message>
<xml_diff>
--- a/Question Sheet.xlsx
+++ b/Question Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shubhammazumdar/Library/Mobile Documents/com~apple~CloudDocs/Level2/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F59C6E-2EBA-CD4F-AFC1-20F6B04D31F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D4294A-8575-D043-9CFE-DEDBCA0F55F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15820" activeTab="1" xr2:uid="{688ABEC1-99B5-A148-B24E-133D3C1DE4DF}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15820" xr2:uid="{688ABEC1-99B5-A148-B24E-133D3C1DE4DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="82">
   <si>
     <t>17th Aug 2022</t>
   </si>
@@ -276,6 +276,12 @@
   </si>
   <si>
     <t>Answers on 6th Sep class</t>
+  </si>
+  <si>
+    <t>Equivalent subarrays</t>
+  </si>
+  <si>
+    <t>Debug your code check answer class</t>
   </si>
 </sst>
 </file>
@@ -685,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD82ACF5-6E46-2A4E-8CDB-3350DDC49501}">
   <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="132" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="132" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1701,8 +1707,13 @@
     </row>
     <row r="31" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
+      <c r="B31" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
+      <c r="D31" s="6" t="s">
+        <v>81</v>
+      </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
@@ -28325,7 +28336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B700801-C5A7-E248-947B-370713DC0001}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Smallest subarray containg all characters of itself
</commit_message>
<xml_diff>
--- a/Question Sheet.xlsx
+++ b/Question Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shubhammazumdar/Library/Mobile Documents/com~apple~CloudDocs/Level2/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27714B87-EFD2-FA46-8E04-1B8D847E5A41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBA267B-56EC-6146-9E22-ACBE4ED59132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15820" xr2:uid="{688ABEC1-99B5-A148-B24E-133D3C1DE4DF}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Dev" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="86">
   <si>
     <t>17th Aug 2022</t>
   </si>
@@ -288,6 +288,12 @@
   </si>
   <si>
     <t>2 test cases failing</t>
+  </si>
+  <si>
+    <t>Smallest subarray with maximum frequency ocurrence of elements</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -718,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD82ACF5-6E46-2A4E-8CDB-3350DDC49501}">
   <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1770,9 +1776,16 @@
     </row>
     <row r="32" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
+      <c r="B32" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="C32" s="4"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="4"/>
+      <c r="D32" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>

</xml_diff>

<commit_message>
Diagonal traversal of a binary tree
</commit_message>
<xml_diff>
--- a/Question Sheet.xlsx
+++ b/Question Sheet.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shubhammazumdar/Library/Mobile Documents/com~apple~CloudDocs/Level2/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71BB75AB-0EBD-CB45-87B3-175BD2D9E8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49A8F14-7CFC-8540-829F-1C48EC99EA77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15820" xr2:uid="{688ABEC1-99B5-A148-B24E-133D3C1DE4DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Dev" sheetId="2" r:id="rId2"/>
+    <sheet name="Self Rev" sheetId="3" r:id="rId2"/>
+    <sheet name="Dev" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="93">
   <si>
     <t>17th Aug 2022</t>
   </si>
@@ -295,6 +296,27 @@
   <si>
     <t>Done</t>
   </si>
+  <si>
+    <t>Constructor of BT</t>
+  </si>
+  <si>
+    <t>Todo</t>
+  </si>
+  <si>
+    <t>Pre in post traversal</t>
+  </si>
+  <si>
+    <t>Level Order Traversal</t>
+  </si>
+  <si>
+    <t>Size, Min, max, height</t>
+  </si>
+  <si>
+    <t>Node to root path</t>
+  </si>
+  <si>
+    <t>Didn't try</t>
+  </si>
 </sst>
 </file>
 
@@ -380,7 +402,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -407,6 +429,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -724,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD82ACF5-6E46-2A4E-8CDB-3350DDC49501}">
   <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2410,7 +2433,7 @@
     </row>
     <row r="52" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4"/>
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="14" t="s">
         <v>48</v>
       </c>
       <c r="C52" s="5" t="s">
@@ -2419,7 +2442,9 @@
       <c r="D52" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E52" s="4"/>
+      <c r="E52" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
@@ -28381,6 +28406,64 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6F2AEBE-F0CB-2146-A21B-E183450199D2}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="59.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B700801-C5A7-E248-947B-370713DC0001}">
   <dimension ref="A1:B1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Left view of a BT
</commit_message>
<xml_diff>
--- a/Question Sheet.xlsx
+++ b/Question Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shubhammazumdar/Library/Mobile Documents/com~apple~CloudDocs/Level2/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49A8F14-7CFC-8540-829F-1C48EC99EA77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D72A4D4-D95F-9C45-91E4-CEC81E5653DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15820" xr2:uid="{688ABEC1-99B5-A148-B24E-133D3C1DE4DF}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="93">
   <si>
     <t>17th Aug 2022</t>
   </si>
@@ -745,10 +745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD82ACF5-6E46-2A4E-8CDB-3350DDC49501}">
-  <dimension ref="A1:Z1006"/>
+  <dimension ref="A1:Z1007"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2524,16 +2524,14 @@
       <c r="Y54" s="4"/>
       <c r="Z54" s="4"/>
     </row>
-    <row r="55" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="4"/>
       <c r="B55" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
-      <c r="C55" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>3</v>
+      <c r="C55" s="4"/>
+      <c r="D55" s="10" t="s">
+        <v>81</v>
       </c>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
@@ -2561,13 +2559,13 @@
     <row r="56" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4"/>
       <c r="B56" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
@@ -2595,7 +2593,7 @@
     <row r="57" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="4"/>
       <c r="B57" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>2</v>
@@ -2629,13 +2627,13 @@
     <row r="58" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4"/>
       <c r="B58" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
@@ -2663,13 +2661,13 @@
     <row r="59" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="4"/>
       <c r="B59" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
@@ -2697,13 +2695,13 @@
     <row r="60" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="4"/>
       <c r="B60" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
@@ -2730,8 +2728,15 @@
     </row>
     <row r="61" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="4"/>
-      <c r="C61" s="4"/>
-      <c r="D61" s="8"/>
+      <c r="B61" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>56</v>
+      </c>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
       <c r="G61" s="4"/>
@@ -2757,9 +2762,6 @@
     </row>
     <row r="62" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="4"/>
-      <c r="B62" s="12" t="s">
-        <v>57</v>
-      </c>
       <c r="C62" s="4"/>
       <c r="D62" s="8"/>
       <c r="E62" s="4"/>
@@ -2787,15 +2789,11 @@
     </row>
     <row r="63" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="4"/>
-      <c r="B63" s="1" t="s">
-        <v>58</v>
+      <c r="B63" s="12" t="s">
+        <v>57</v>
       </c>
-      <c r="C63" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D63" s="8" t="s">
-        <v>3</v>
-      </c>
+      <c r="C63" s="4"/>
+      <c r="D63" s="8"/>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
@@ -2822,13 +2820,13 @@
     <row r="64" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4"/>
       <c r="B64" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
@@ -2856,13 +2854,13 @@
     <row r="65" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="4"/>
       <c r="B65" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
@@ -2890,13 +2888,13 @@
     <row r="66" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="4"/>
       <c r="B66" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
@@ -2923,8 +2921,15 @@
     </row>
     <row r="67" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="4"/>
-      <c r="C67" s="4"/>
-      <c r="D67" s="8"/>
+      <c r="B67" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>60</v>
+      </c>
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
       <c r="G67" s="4"/>
@@ -2950,9 +2955,6 @@
     </row>
     <row r="68" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="4"/>
-      <c r="B68" s="13" t="s">
-        <v>63</v>
-      </c>
       <c r="C68" s="4"/>
       <c r="D68" s="8"/>
       <c r="E68" s="4"/>
@@ -2980,15 +2982,11 @@
     </row>
     <row r="69" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4"/>
-      <c r="B69" s="1" t="s">
-        <v>64</v>
+      <c r="B69" s="13" t="s">
+        <v>63</v>
       </c>
-      <c r="C69" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D69" s="8" t="s">
-        <v>3</v>
-      </c>
+      <c r="C69" s="4"/>
+      <c r="D69" s="8"/>
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
@@ -3015,13 +3013,13 @@
     <row r="70" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4"/>
       <c r="B70" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>66</v>
+        <v>3</v>
       </c>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
@@ -3049,13 +3047,13 @@
     <row r="71" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="4"/>
       <c r="B71" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
@@ -3083,13 +3081,13 @@
     <row r="72" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="4"/>
       <c r="B72" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
@@ -3117,13 +3115,13 @@
     <row r="73" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="4"/>
       <c r="B73" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>70</v>
+        <v>13</v>
       </c>
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
@@ -3151,13 +3149,13 @@
     <row r="74" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="4"/>
       <c r="B74" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
@@ -3184,8 +3182,15 @@
     </row>
     <row r="75" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="4"/>
-      <c r="C75" s="4"/>
-      <c r="D75" s="8"/>
+      <c r="B75" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>72</v>
+      </c>
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
       <c r="G75" s="4"/>
@@ -3211,12 +3216,7 @@
     </row>
     <row r="76" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="4"/>
-      <c r="B76" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>2</v>
-      </c>
+      <c r="C76" s="4"/>
       <c r="D76" s="8"/>
       <c r="E76" s="4"/>
       <c r="F76" s="4"/>
@@ -3244,9 +3244,11 @@
     <row r="77" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="4"/>
       <c r="B77" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
-      <c r="C77" s="4"/>
+      <c r="C77" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="D77" s="8"/>
       <c r="E77" s="4"/>
       <c r="F77" s="4"/>
@@ -3274,7 +3276,7 @@
     <row r="78" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="4"/>
       <c r="B78" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C78" s="4"/>
       <c r="D78" s="8"/>
@@ -3304,7 +3306,7 @@
     <row r="79" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="4"/>
       <c r="B79" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C79" s="4"/>
       <c r="D79" s="8"/>
@@ -3333,6 +3335,9 @@
     </row>
     <row r="80" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="4"/>
+      <c r="B80" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="C80" s="4"/>
       <c r="D80" s="8"/>
       <c r="E80" s="4"/>
@@ -28360,6 +28365,33 @@
       <c r="Y1006" s="4"/>
       <c r="Z1006" s="4"/>
     </row>
+    <row r="1007" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1007" s="4"/>
+      <c r="C1007" s="4"/>
+      <c r="D1007" s="8"/>
+      <c r="E1007" s="4"/>
+      <c r="F1007" s="4"/>
+      <c r="G1007" s="4"/>
+      <c r="H1007" s="4"/>
+      <c r="I1007" s="4"/>
+      <c r="J1007" s="4"/>
+      <c r="K1007" s="4"/>
+      <c r="L1007" s="4"/>
+      <c r="M1007" s="4"/>
+      <c r="N1007" s="4"/>
+      <c r="O1007" s="4"/>
+      <c r="P1007" s="4"/>
+      <c r="Q1007" s="4"/>
+      <c r="R1007" s="4"/>
+      <c r="S1007" s="4"/>
+      <c r="T1007" s="4"/>
+      <c r="U1007" s="4"/>
+      <c r="V1007" s="4"/>
+      <c r="W1007" s="4"/>
+      <c r="X1007" s="4"/>
+      <c r="Y1007" s="4"/>
+      <c r="Z1007" s="4"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C13" r:id="rId1" display="https://nados.io/question/count-of-subarrays-with-equal-number-of-zeroes-and-ones" xr:uid="{56B39D9D-F484-F746-9FCC-20F1666E8089}"/>
@@ -28383,23 +28415,23 @@
     <hyperlink ref="C50" r:id="rId19" display="https://practice.geeksforgeeks.org/problems/binary-tree-to-dll/1" xr:uid="{D6150988-5F2F-D84B-9393-AC61278C2B80}"/>
     <hyperlink ref="C51" r:id="rId20" display="https://practice.geeksforgeeks.org/problems/burning-tree/1" xr:uid="{B2AA558E-FA27-4745-9587-F69F48FE6C4F}"/>
     <hyperlink ref="C52" r:id="rId21" display="https://leetcode.com/problems/house-robber-iii/" xr:uid="{D2ADC581-2A9E-6F42-8C90-15F560D29050}"/>
-    <hyperlink ref="C55" r:id="rId22" display="https://practice.geeksforgeeks.org/problems/left-view-of-binary-tree/1" xr:uid="{352901EA-708C-E345-8B07-35342EC80B16}"/>
-    <hyperlink ref="C56" r:id="rId23" display="https://practice.geeksforgeeks.org/problems/right-view-of-binary-tree/1" xr:uid="{23C8BF3A-D0F9-6F4E-BF3B-D000978E2A65}"/>
-    <hyperlink ref="C57" r:id="rId24" display="https://leetcode.com/problems/binary-tree-right-side-view/" xr:uid="{B95791CD-94D1-9C49-91ED-A12FEC662880}"/>
-    <hyperlink ref="C58" r:id="rId25" display="https://practice.geeksforgeeks.org/problems/top-view-of-binary-tree/1" xr:uid="{C3618A33-1AC7-8840-8855-5D95193F0D74}"/>
-    <hyperlink ref="C59" r:id="rId26" display="https://practice.geeksforgeeks.org/problems/bottom-view-of-binary-tree/1" xr:uid="{7A02D06B-655D-3245-AB5C-FAB2BC32750A}"/>
-    <hyperlink ref="C60" r:id="rId27" display="https://leetcode.com/problems/vertical-order-traversal-of-a-binary-tree/" xr:uid="{AB7C35B9-E5BA-5A46-B632-E4C5C5EDA7C5}"/>
-    <hyperlink ref="C63" r:id="rId28" display="https://leetcode.com/problems/recover-binary-search-tree/" xr:uid="{B62633A5-9C0D-1349-940F-8996FB8D52C0}"/>
-    <hyperlink ref="C64" r:id="rId29" display="https://leetcode.com/problems/maximum-width-of-binary-tree/" xr:uid="{0EF776BC-79DB-8F4C-A6B3-3C41F10D0C99}"/>
-    <hyperlink ref="C65" r:id="rId30" display="https://practice.geeksforgeeks.org/problems/boundary-traversal-of-binary-tree/1" xr:uid="{2DA67615-C78B-0A4A-A100-1245B6C1F33D}"/>
-    <hyperlink ref="C66" r:id="rId31" display="https://practice.geeksforgeeks.org/problems/diagonal-traversal-of-binary-tree/1" xr:uid="{6C0083EA-D9A3-DE4F-96A2-CBB805FACAA2}"/>
-    <hyperlink ref="C69" r:id="rId32" display="https://leetcode.com/problems/construct-binary-tree-from-preorder-and-inorder-traversal/" xr:uid="{5ADFF790-5F13-EC4D-86F7-619868333EB4}"/>
-    <hyperlink ref="C70" r:id="rId33" display="https://leetcode.com/problems/construct-binary-tree-from-inorder-and-postorder-traversal/" xr:uid="{0F38431C-CC31-A142-BE0B-DB8391ACFD00}"/>
-    <hyperlink ref="C71" r:id="rId34" display="https://practice.geeksforgeeks.org/problems/construct-tree-from-inorder-and-levelorder/1" xr:uid="{E59B0279-83B0-0749-B933-4F96E9F7CC51}"/>
-    <hyperlink ref="C72" r:id="rId35" display="https://practice.geeksforgeeks.org/problems/convert-level-order-traversal-to-bst/1" xr:uid="{7D0DE4AC-4969-1641-8AC6-D714DD283541}"/>
-    <hyperlink ref="C73" r:id="rId36" display="https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-search-tree/" xr:uid="{04C325E7-9976-4C43-B32E-CBCCDB933775}"/>
-    <hyperlink ref="C74" r:id="rId37" display="https://leetcode.com/problems/validate-binary-search-tree/" xr:uid="{88C7D357-D22F-D844-AAB8-142B6AA3789D}"/>
-    <hyperlink ref="C76" r:id="rId38" display="https://leetcode.com/problems/populating-next-right-pointers-in-each-node/" xr:uid="{95D944FD-B1B0-BF46-99BA-F0440C4722CC}"/>
+    <hyperlink ref="C56" r:id="rId22" display="https://practice.geeksforgeeks.org/problems/left-view-of-binary-tree/1" xr:uid="{352901EA-708C-E345-8B07-35342EC80B16}"/>
+    <hyperlink ref="C57" r:id="rId23" display="https://practice.geeksforgeeks.org/problems/right-view-of-binary-tree/1" xr:uid="{23C8BF3A-D0F9-6F4E-BF3B-D000978E2A65}"/>
+    <hyperlink ref="C58" r:id="rId24" display="https://leetcode.com/problems/binary-tree-right-side-view/" xr:uid="{B95791CD-94D1-9C49-91ED-A12FEC662880}"/>
+    <hyperlink ref="C59" r:id="rId25" display="https://practice.geeksforgeeks.org/problems/top-view-of-binary-tree/1" xr:uid="{C3618A33-1AC7-8840-8855-5D95193F0D74}"/>
+    <hyperlink ref="C60" r:id="rId26" display="https://practice.geeksforgeeks.org/problems/bottom-view-of-binary-tree/1" xr:uid="{7A02D06B-655D-3245-AB5C-FAB2BC32750A}"/>
+    <hyperlink ref="C61" r:id="rId27" display="https://leetcode.com/problems/vertical-order-traversal-of-a-binary-tree/" xr:uid="{AB7C35B9-E5BA-5A46-B632-E4C5C5EDA7C5}"/>
+    <hyperlink ref="C64" r:id="rId28" display="https://leetcode.com/problems/recover-binary-search-tree/" xr:uid="{B62633A5-9C0D-1349-940F-8996FB8D52C0}"/>
+    <hyperlink ref="C65" r:id="rId29" display="https://leetcode.com/problems/maximum-width-of-binary-tree/" xr:uid="{0EF776BC-79DB-8F4C-A6B3-3C41F10D0C99}"/>
+    <hyperlink ref="C66" r:id="rId30" display="https://practice.geeksforgeeks.org/problems/boundary-traversal-of-binary-tree/1" xr:uid="{2DA67615-C78B-0A4A-A100-1245B6C1F33D}"/>
+    <hyperlink ref="C67" r:id="rId31" display="https://practice.geeksforgeeks.org/problems/diagonal-traversal-of-binary-tree/1" xr:uid="{6C0083EA-D9A3-DE4F-96A2-CBB805FACAA2}"/>
+    <hyperlink ref="C70" r:id="rId32" display="https://leetcode.com/problems/construct-binary-tree-from-preorder-and-inorder-traversal/" xr:uid="{5ADFF790-5F13-EC4D-86F7-619868333EB4}"/>
+    <hyperlink ref="C71" r:id="rId33" display="https://leetcode.com/problems/construct-binary-tree-from-inorder-and-postorder-traversal/" xr:uid="{0F38431C-CC31-A142-BE0B-DB8391ACFD00}"/>
+    <hyperlink ref="C72" r:id="rId34" display="https://practice.geeksforgeeks.org/problems/construct-tree-from-inorder-and-levelorder/1" xr:uid="{E59B0279-83B0-0749-B933-4F96E9F7CC51}"/>
+    <hyperlink ref="C73" r:id="rId35" display="https://practice.geeksforgeeks.org/problems/convert-level-order-traversal-to-bst/1" xr:uid="{7D0DE4AC-4969-1641-8AC6-D714DD283541}"/>
+    <hyperlink ref="C74" r:id="rId36" display="https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-search-tree/" xr:uid="{04C325E7-9976-4C43-B32E-CBCCDB933775}"/>
+    <hyperlink ref="C75" r:id="rId37" display="https://leetcode.com/problems/validate-binary-search-tree/" xr:uid="{88C7D357-D22F-D844-AAB8-142B6AA3789D}"/>
+    <hyperlink ref="C77" r:id="rId38" display="https://leetcode.com/problems/populating-next-right-pointers-in-each-node/" xr:uid="{95D944FD-B1B0-BF46-99BA-F0440C4722CC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>